<commit_message>
JSON Data: Updating more of the JSON data. adding born die date strings and places of burial and births
</commit_message>
<xml_diff>
--- a/s2cAllRawDataExcel.xlsx
+++ b/s2cAllRawDataExcel.xlsx
@@ -521,7 +521,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -572,8 +572,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -856,10 +859,10 @@
   <dimension ref="A1:G274"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -896,7 +899,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" ht="409" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
@@ -942,442 +945,442 @@
     </row>
     <row r="4" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="B4" s="12"/>
-      <c r="C4" s="9" t="s">
-        <v>40</v>
-      </c>
+      <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="409" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="12">
-        <v>4192</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>80</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="2" t="s">
-        <v>79</v>
-      </c>
+      <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="289" x14ac:dyDescent="0.25">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>5</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B6" s="12"/>
       <c r="C6" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>7</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="409" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="12">
+        <v>4192</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" ht="289" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="409" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B10" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C10" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E10" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="409" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" ht="409.6" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>22</v>
-      </c>
+      <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="12">
-        <v>10608</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="B11" s="12"/>
       <c r="C11" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="409" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="12">
-        <v>15662</v>
+        <v>57</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="409" x14ac:dyDescent="0.35">
+      <c r="G12" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>24</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B13" s="12"/>
       <c r="C13" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="409" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>63</v>
+        <v>84</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>22</v>
       </c>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="62" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>41</v>
+        <v>16</v>
+      </c>
+      <c r="B15" s="12">
+        <v>10608</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" ht="248" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="B16" s="12">
+        <v>15662</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>46</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D16" s="9"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" ht="409" x14ac:dyDescent="0.35">
-      <c r="A17" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>69</v>
-      </c>
+    <row r="17" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+      <c r="A17" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="12"/>
       <c r="C17" s="9" t="s">
         <v>70</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="310" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" ht="409" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" s="12"/>
+        <v>12</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="C18" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="9"/>
+        <v>36</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="E18" s="2" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" ht="93" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="409" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+        <v>54</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="9"/>
+        <v>39</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>40</v>
+      </c>
       <c r="D20" s="9"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="124" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="B21" s="12"/>
-      <c r="C21" s="9"/>
+      <c r="C21" s="9" t="s">
+        <v>110</v>
+      </c>
       <c r="D21" s="9"/>
-      <c r="E21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" ht="248" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B22" s="12"/>
+        <v>34</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="C22" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F22" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" ht="155" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="62" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B23" s="12"/>
-      <c r="C23" s="9"/>
+      <c r="C23" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="D23" s="9"/>
       <c r="E23" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="62" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B24" s="12"/>
-      <c r="C24" s="9"/>
+      <c r="C24" s="9" t="s">
+        <v>109</v>
+      </c>
       <c r="D24" s="9"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="9" t="s">
         <v>70</v>
       </c>
       <c r="D25" s="9"/>
-      <c r="E25" s="2" t="s">
-        <v>100</v>
-      </c>
+      <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" ht="62" x14ac:dyDescent="0.35">
-      <c r="A26" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B26" s="12"/>
+    <row r="26" spans="1:7" ht="409" x14ac:dyDescent="0.35">
+      <c r="A26" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>69</v>
+      </c>
       <c r="C26" s="9" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="248" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="9" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="2" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="310" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="9" t="s">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="D28" s="9"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="93" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="B29" s="12"/>
+        <v>37</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>48</v>
+      </c>
       <c r="C29" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" s="9"/>
+        <v>38</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="155" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B30" s="12"/>
-      <c r="C30" s="9" t="s">
-        <v>108</v>
-      </c>
+      <c r="C30" s="9"/>
       <c r="D30" s="9"/>
-      <c r="E30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
@@ -3581,14 +3584,14 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:G1">
-    <sortState ref="A2:G19">
-      <sortCondition ref="A1:A19"/>
+    <sortState ref="A2:G31">
+      <sortCondition ref="A1:A31"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="G13" r:id="rId1"/>
-    <hyperlink ref="G8" r:id="rId2"/>
-    <hyperlink ref="G5" r:id="rId3"/>
+    <hyperlink ref="G18" r:id="rId1"/>
+    <hyperlink ref="G12" r:id="rId2"/>
+    <hyperlink ref="G7" r:id="rId3"/>
     <hyperlink ref="G2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added new images and also fixed json text. Changed detailvc image fit to Aspect Fit which will make things look better.
</commit_message>
<xml_diff>
--- a/s2cAllRawDataExcel.xlsx
+++ b/s2cAllRawDataExcel.xlsx
@@ -859,10 +859,10 @@
   <dimension ref="A1:G274"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Model: Added a whole bunch of face image assets and people data
</commit_message>
<xml_diff>
--- a/s2cAllRawDataExcel.xlsx
+++ b/s2cAllRawDataExcel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/terrybu/Desktop/Projects/Setbacks to Comebacks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/terrybu/Projects/Setbacks to Comebacks/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="115">
   <si>
     <t>Name</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>Depression, Suicidal Thoughts</t>
-  </si>
-  <si>
-    <t>Little is known about the fact that he tried to kill himself as a child</t>
   </si>
   <si>
     <t>Muhammad</t>
@@ -270,9 +267,6 @@
     <t>Late Bloomer</t>
   </si>
   <si>
-    <t>The Wrights Brothers</t>
-  </si>
-  <si>
     <t>No Formal Education</t>
   </si>
   <si>
@@ -309,9 +303,6 @@
 The moral: it sometimes pays an agency to be imaginative and unorthodox in hiring.'</t>
   </si>
   <si>
-    <t>Dropped out of college, No Formal Education, Late Bloomer, Career Hopping During Youth</t>
-  </si>
-  <si>
     <t>Setbacks</t>
   </si>
   <si>
@@ -416,6 +407,21 @@
   </si>
   <si>
     <t>Winston Churchill</t>
+  </si>
+  <si>
+    <t>The Wright Brothers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Little is known about the fact that MLK Jr had depression. The fact that Dr King was severely down, even clinically depressed, has been established by prior historians. Most observers rationalize King's depression by describing the many stresses of his life: the civil rights movement was in danger indeed—threatened by the Black Power movement on its left and, ever since Dr King came out strongly against the Vietnam War, deserted by President Lyndon Johnson and the liberal Democratic establishment on its right. King's poll numbers had fallen drastically, such that less than one third of the American public had a positive opinion of him. He was receiving more and more death threats. He knew he was risking his life daily, and for what? No one seemed to be listening to him anymore. </t>
+  </si>
+  <si>
+    <t>Ellen DeGeneres</t>
+  </si>
+  <si>
+    <t>Dropped out of school, Late Bloomer, Changed Jobs Multiple Times</t>
+  </si>
+  <si>
+    <t>Dropped out of college, No Formal Education, Late Bloomer, Changed Jobs multiple times</t>
   </si>
 </sst>
 </file>
@@ -859,10 +865,10 @@
   <dimension ref="A1:G274"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -884,7 +890,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>10</v>
@@ -904,48 +910,48 @@
         <v>14</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="E2" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="409" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="E3" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="G3" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="9"/>
@@ -956,7 +962,7 @@
     </row>
     <row r="5" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="9"/>
@@ -967,11 +973,11 @@
     </row>
     <row r="6" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="2"/>
@@ -980,26 +986,26 @@
     </row>
     <row r="7" spans="1:7" ht="409" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B7" s="12">
         <v>4192</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="9"/>
@@ -1016,16 +1022,16 @@
         <v>5</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>7</v>
@@ -1033,30 +1039,30 @@
     </row>
     <row r="10" spans="1:7" ht="409" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="2"/>
@@ -1065,32 +1071,32 @@
     </row>
     <row r="12" spans="1:7" ht="409" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="2"/>
@@ -1108,17 +1114,17 @@
         <v>13</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="409" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>16</v>
       </c>
@@ -1129,23 +1135,23 @@
         <v>17</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>18</v>
+        <v>111</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="12">
         <v>15662</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="2"/>
@@ -1154,15 +1160,15 @@
     </row>
     <row r="17" spans="1:7" ht="124" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1172,54 +1178,54 @@
         <v>12</v>
       </c>
       <c r="B18" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="409" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="F19" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>40</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="2"/>
@@ -1228,60 +1234,60 @@
     </row>
     <row r="21" spans="1:7" ht="124" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" ht="248" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>15</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" ht="62" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" ht="62" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="2"/>
@@ -1290,11 +1296,11 @@
     </row>
     <row r="25" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="2"/>
@@ -1303,69 +1309,69 @@
     </row>
     <row r="26" spans="1:7" ht="409" x14ac:dyDescent="0.35">
       <c r="A26" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B26" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>69</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>70</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="248" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="310" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" ht="93" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="D29" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>49</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -1373,20 +1379,20 @@
     </row>
     <row r="30" spans="1:7" ht="155" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
       <c r="E30" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="9"/>
@@ -1395,10 +1401,14 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A32" s="9"/>
+    <row r="32" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+      <c r="A32" s="9" t="s">
+        <v>112</v>
+      </c>
       <c r="B32" s="12"/>
-      <c r="C32" s="9"/>
+      <c r="C32" s="9" t="s">
+        <v>113</v>
+      </c>
       <c r="D32" s="9"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>

</xml_diff>

<commit_message>
updating biography for many people like Edison, Einstein, etc
</commit_message>
<xml_diff>
--- a/s2cAllRawDataExcel.xlsx
+++ b/s2cAllRawDataExcel.xlsx
@@ -865,10 +865,10 @@
   <dimension ref="A1:G274"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>